<commit_message>
Update DPE for red blood cell count var
</commit_message>
<xml_diff>
--- a/data_processing_elements-BCS.xlsx
+++ b/data_processing_elements-BCS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B1E053-CBF5-43BA-8D8C-967392EF2C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90276CDF-D91A-4EE3-ABAE-81BF440F9B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2A6783BB-5B5E-40A9-959B-24C52A32495F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A6783BB-5B5E-40A9-959B-24C52A32495F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="572">
   <si>
     <t>BCS</t>
   </si>
@@ -2910,6 +2910,9 @@
 (B10MEDLNGW_1 %in% c(-9, -8, -1)) | (B10MEDLNGW_2 %in% c(-9, -8, -1)) | (B10MEDLNGW_3 %in% c(-9, -8, -1)) | (B10MEDLNGW_4 %in% c(-9, -8, -1)) | (B10MEDLNGW_5 %in% c(-9, -8, -1)) | (B10MEDLNGW_6 %in% c(-9, -8, -1)) | (B10MEDLNGW_7 %in% c(-9, -8, -1)) | (B10MEDLNGW_8 %in% c(-9, -8, -1)) | (B10MEDLNGW_9 %in% c(-9, -8, -1)) ~ NA_integer_;
 ELSE ~ 0L)</t>
   </si>
+  <si>
+    <t>direct_mapping</t>
+  </si>
 </sst>
 </file>
 
@@ -3019,7 +3022,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3337,11 +3340,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5E8CE2-4CDD-4679-8B68-FC70B285017D}">
   <dimension ref="A1:W84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R71" workbookViewId="0">
-      <selection activeCell="W75" sqref="W75"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="31.42578125" style="1" customWidth="1"/>
@@ -5019,16 +5022,16 @@
         <v>248</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>249</v>
+        <v>12</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>95</v>
+        <v>571</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>95</v>
+        <v>571</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>